<commit_message>
bento age slider, INS fixes
</commit_message>
<xml_diff>
--- a/InputFiles/INS/TC01_INS_Filter_Doc-CCG.xlsx
+++ b/InputFiles/INS/TC01_INS_Filter_Doc-CCG.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation Latest\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\August\Commons_Automation\InputFiles\INS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B3BD8E-4659-4E14-AC30-86990DF64B9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198BECBA-2036-4CBD-99FB-D40B5F09353D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -67,6 +67,29 @@
     <t>PatentsTab</t>
   </si>
   <si>
+    <t>MATCH (p:program)&lt;--(pr:project)
+where pr.lead_doc='CCG'
+OPTIONAL MATCH (pr)&lt;--(pub:publication)
+OPTIONAL MATCH (ct:clinical_trial)
+WHERE EXISTS((pr)&lt;--(pub)&lt;--(ct)) OR EXISTS((pr)&lt;--(ct))
+OPTIONAL MATCH (pr)&lt;--(pat)
+WHERE pat:patent_application OR pat:granted_patent
+OPTIONAL MATCH (pr)&lt;-[*1..2]-(dt)
+WHERE dt:sra OR dt:dbgap OR dt:geo
+WITH p, pr, pub, ct, pat, dt
+RETURN
+COUNT(DISTINCT p.program_id) AS Programs,
+COUNT(DISTINCT pr.queried_project_id) AS Projects,
+COUNT(DISTINCT pr.project_id) AS Grants,
+COUNT(DISTINCT pub.publication_id) AS Publications,
+COUNT(DISTINCT dt.accession) AS Datasets,
+COUNT(DISTINCT ct.clinical_trial_id) AS `Clinical Trials`,
+COUNT(DISTINCT pat.patent_id) AS Patents</t>
+  </si>
+  <si>
+    <t>GrantsTab</t>
+  </si>
+  <si>
     <t>MATCH (pr:project)--&gt;(pgm:program)
 where pr.lead_doc='CCG'
 WITH DISTINCT pr, pgm
@@ -81,7 +104,9 @@
 SUBSTRING(pr.project_id, 1, 3) AS `Activity code`,
 "$" + apoc.number.format(toInteger(pr.award_amount)) AS `Award Amount`,
 coalesce(pr.project_end_date, '') AS `Project End Date`,
-coalesce(pr.fiscal_year,'')AS `Fiscal Year`</t>
+coalesce(pr.fiscal_year,'')AS `Fiscal Year`
+order by pr.project_id ASC
+LIMIT 100</t>
   </si>
   <si>
     <t>MATCH (pr:project)&lt;--(:publication)&lt;--(dt)
@@ -102,36 +127,21 @@
     COALESCE(dt.release_date,'') AS `Release Date`,
     COALESCE(dt.registration_date,'') AS `Registration Date`
     order by Accession ASC
-MATCH (dt)
-            WHERE (dt:geo OR dt:sra OR dt:dbgap)
-             MATCH (p:program)&lt;--(pr:project)&lt;--()&lt;--(dt)
-            RETURN DISTINCT
-          dt.accession AS Accession,
-          COALESCE (pr.queried_project_id,'') AS `Project IDs`,
-          CASE LABELS(dt)[0]
-              WHEN 'geo' THEN 'GEO'
-              WHEN 'sra' THEN 'SRA'
-              WHEN 'dbgap' THEN 'dbGaP' END AS Type,
-          COALESCE(dt.title, dt.study_title) AS Title,
-         COALESCE (dt.submission_date,'') AS `Submission Date`,
-          coalesce (dt.last_update_date,'') AS `Last Update Date`,
-          COALESCE (dt.release_date,'') AS `Release Date`,
-         COALESCE (dt.registration_date,'') AS `Registration Date`</t>
-  </si>
-  <si>
-    <t>MATCH (pr:project)&lt;--(pub:publication)
-MATCH (pr2:project)&lt;--(pub:publication)
+Limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (pr:project)&lt;--()&lt;--(ct:clinical_trial)
+MATCH (pr2:project)&lt;--()&lt;--(ct:clinical_trial)
     WHERE pr.lead_doc='CCG'
-WITH pub, COLLECT(DISTINCT pr.queried_project_id)+COLLECT(DISTINCT pr2.queried_project_id) AS prids
+WITH ct, COLLECT(DISTINCT pr.queried_project_id)+COLLECT(DISTINCT pr2.queried_project_id) AS prids
 RETURN DISTINCT
-    COALESCE(pub.publication_id,'') AS `PubMed ID`,
+    COALESCE(ct.clinical_trial_id,'') AS `Clinical Trial ID`,
     apoc.text.join(apoc.coll.toSet(prids),", ") AS `Project IDs`,
-    pub.title AS Title,
-    pub.authors AS Authors,
-    pub.citation_count AS `Citation Count`,
-    pub.relative_citation_ratio AS `Relative Citation Ratio`,
-    pub.publish_date AS `Publication Date`
-order by `PubMed ID` ASC</t>
+    ct.title AS Title,
+    ct.last_update_date AS `Last Update Date`,
+    ct.recruitment_status AS `Recruitment Status`
+order by `Clinical Trial ID` ASC
+LIMIT 100</t>
   </si>
   <si>
     <t>MATCH (pr:project)&lt;--(pat)
@@ -145,47 +155,20 @@
 order by `Patent ID` ASC</t>
   </si>
   <si>
-    <t>MATCH (pr:project)&lt;--(:publication)&lt;--(dt)
-MATCH (pr2:project)&lt;--(:publication)&lt;--(dt)
-    WHERE (dt:geo OR dt:sra OR dt:dbgap) AND pr.lead_doc='CCG'
-WITH dt, COLLECT(DISTINCT pr.queried_project_id)+COLLECT(DISTINCT pr2.queried_project_id) AS prids
+    <t>MATCH (pr:project)&lt;--(pub:publication)
+MATCH (pr2:project)&lt;--(pub:publication)
+    WHERE pr.lead_doc='CCG'
+WITH pub, apoc.coll.reverse(apoc.coll.sort(COLLECT(DISTINCT pr.queried_project_id)+COLLECT(DISTINCT pr2.queried_project_id) )) AS prids
 RETURN DISTINCT
-    COALESCE(dt.accession,'') AS Accession,
+    COALESCE(pub.publication_id,'') AS `PubMed ID`,
     apoc.text.join(apoc.coll.toSet(prids),", ") AS `Project IDs`,
-    CASE LABELS(dt)[0]
-        WHEN 'geo' THEN 'GEO'
-        WHEN 'sra' THEN 'SRA'
-        WHEN 'dbgap' THEN 'dbGaP'
-    END AS Type,
-    COALESCE(dt.title, dt.study_title,'') AS Title,
-    COALESCE(dt.submission_date,'') AS `Submission Date`,
-    COALESCE(dt.last_update_date,'') AS `Last Update Date`,
-    COALESCE(dt.release_date,'') AS `Release Date`,
-    COALESCE(dt.registration_date,'') AS `Registration Date`
-    order by Accession ASC</t>
-  </si>
-  <si>
-    <t>MATCH (p:program)&lt;--(pr:project)
-where pr.lead_doc='CCG'
-OPTIONAL MATCH (pr)&lt;--(pub:publication)
-OPTIONAL MATCH (ct:clinical_trial)
-WHERE EXISTS((pr)&lt;--(pub)&lt;--(ct)) OR EXISTS((pr)&lt;--(ct))
-OPTIONAL MATCH (pr)&lt;--(pat)
-WHERE pat:patent_application OR pat:granted_patent
-OPTIONAL MATCH (pr)&lt;-[*1..2]-(dt)
-WHERE dt:sra OR dt:dbgap OR dt:geo
-WITH p, pr, pub, ct, pat, dt
-RETURN
-COUNT(DISTINCT p.program_id) AS Programs,
-COUNT(DISTINCT pr.queried_project_id) AS Projects,
-COUNT(DISTINCT pr.project_id) AS Grants,
-COUNT(DISTINCT pub.publication_id) AS Publications,
-COUNT(DISTINCT dt.accession) AS Datasets,
-COUNT(DISTINCT ct.clinical_trial_id) AS `Clinical Trials`,
-COUNT(DISTINCT pat.patent_id) AS Patents</t>
-  </si>
-  <si>
-    <t>GrantsTab</t>
+    pub.title AS Title,
+    pub.authors AS Authors,
+    pub.citation_count AS `Citation Count`,
+    pub.relative_citation_ratio AS `Relative Citation Ratio`,
+    pub.publish_date AS `Publication Date`
+order by `PubMed ID` ASC
+Limit 100</t>
   </si>
 </sst>
 </file>
@@ -558,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,13 +573,13 @@
     </row>
     <row r="2" spans="1:5" ht="270" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D2" t="s">
         <v>5</v>
@@ -605,15 +588,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="390" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="270" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
         <v>5</v>
@@ -622,15 +605,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="300" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -639,7 +622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="270" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -647,7 +630,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
@@ -661,10 +644,10 @@
         <v>10</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>

</xml_diff>